<commit_message>
Updating for new data
</commit_message>
<xml_diff>
--- a/Apps/YouTubeAnalysis/Analysis/Step03_GroupByClassification.xlsx
+++ b/Apps/YouTubeAnalysis/Analysis/Step03_GroupByClassification.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <workbookPr/>
   <bookViews>
     <workbookView activeTab="0"/>
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="17" uniqueCount="17">
   <si>
     <t>Classification</t>
   </si>
@@ -43,12 +43,33 @@
   </si>
   <si>
     <t>ClassVideoDuration_hr</t>
+  </si>
+  <si>
+    <t>ClassNumberVideos_percentage</t>
+  </si>
+  <si>
+    <t>ClassViews_percentage</t>
+  </si>
+  <si>
+    <t>ClassWatchTime_hr_percentage</t>
+  </si>
+  <si>
+    <t>ClassSubscribers_percentage</t>
+  </si>
+  <si>
+    <t>ClassRevenue_USD_percentage</t>
+  </si>
+  <si>
+    <t>ClassImpressions_percentage</t>
+  </si>
+  <si>
+    <t>ClassVideoDuration_hr_percentage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -87,8 +108,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.85546875" customWidth="true"/>
@@ -99,6 +123,13 @@
     <col min="6" max="6" width="18" customWidth="true"/>
     <col min="7" max="7" width="16.28515625" customWidth="true"/>
     <col min="8" max="8" width="21.42578125" customWidth="true"/>
+    <col min="9" max="9" width="30" customWidth="true"/>
+    <col min="10" max="10" width="22" customWidth="true"/>
+    <col min="11" max="11" width="29.42578125" customWidth="true"/>
+    <col min="12" max="12" width="26.7109375" customWidth="true"/>
+    <col min="13" max="13" width="29" customWidth="true"/>
+    <col min="14" max="14" width="27.28515625" customWidth="true"/>
+    <col min="15" max="15" width="32.42578125" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -126,31 +157,73 @@
       <c r="H1" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="I1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="0">
-        <v>177</v>
+        <v>206</v>
       </c>
       <c r="C2" s="0">
-        <v>4410530</v>
+        <v>5354513</v>
       </c>
       <c r="D2" s="0">
-        <v>403862.69469999999</v>
+        <v>484651.17839999998</v>
       </c>
       <c r="E2" s="0">
-        <v>42121</v>
+        <v>51257</v>
       </c>
       <c r="F2" s="0">
-        <v>18162.893</v>
+        <v>21946.979000000003</v>
       </c>
       <c r="G2" s="0">
-        <v>54954916</v>
+        <v>68645276</v>
       </c>
       <c r="H2" s="0">
-        <v>130.35805555555555</v>
+        <v>142.53555555555556</v>
+      </c>
+      <c r="I2" s="0">
+        <v>55.826558265582662</v>
+      </c>
+      <c r="J2" s="0">
+        <v>53.04537362149977</v>
+      </c>
+      <c r="K2" s="0">
+        <v>66.755678300428826</v>
+      </c>
+      <c r="L2" s="0">
+        <v>81.351278429380855</v>
+      </c>
+      <c r="M2" s="0">
+        <v>38.107830417405204</v>
+      </c>
+      <c r="N2" s="0">
+        <v>59.112571152881586</v>
+      </c>
+      <c r="O2" s="0">
+        <v>79.04625902527772</v>
       </c>
     </row>
     <row r="3">
@@ -158,25 +231,46 @@
         <v>2</v>
       </c>
       <c r="B3" s="0">
-        <v>147</v>
+        <v>163</v>
       </c>
       <c r="C3" s="0">
-        <v>3517092</v>
+        <v>4739700</v>
       </c>
       <c r="D3" s="0">
-        <v>181381.60940000002</v>
+        <v>241356.24260000003</v>
       </c>
       <c r="E3" s="0">
-        <v>9126</v>
+        <v>11750</v>
       </c>
       <c r="F3" s="0">
-        <v>26369.695999999996</v>
+        <v>35644.804000000004</v>
       </c>
       <c r="G3" s="0">
-        <v>39470883</v>
+        <v>47481082</v>
       </c>
       <c r="H3" s="0">
-        <v>35.647500000000001</v>
+        <v>37.783611111111114</v>
+      </c>
+      <c r="I3" s="0">
+        <v>44.173441734417345</v>
+      </c>
+      <c r="J3" s="0">
+        <v>46.954626378500237</v>
+      </c>
+      <c r="K3" s="0">
+        <v>33.244321699571174</v>
+      </c>
+      <c r="L3" s="0">
+        <v>18.648721570619138</v>
+      </c>
+      <c r="M3" s="0">
+        <v>61.892169582594789</v>
+      </c>
+      <c r="N3" s="0">
+        <v>40.887428847118414</v>
+      </c>
+      <c r="O3" s="0">
+        <v>20.953740974722294</v>
       </c>
     </row>
   </sheetData>

</xml_diff>